<commit_message>
Frontend - i18n - Translations - Make sure tokens are same in all translations, Fix AR
</commit_message>
<xml_diff>
--- a/frontend/src/i18n/Translations Master.xlsx
+++ b/frontend/src/i18n/Translations Master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://logrhythm-my.sharepoint.com/personal/tony_masse_logrhythm_com/Documents/Tony.Masse/Projets/20210331.EZ-Cloud on Legacy SIEM/EZ-Cloud/frontend/src/i18n/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="412" documentId="8_{4939A0CD-BDFC-4EBB-81BD-8799C6D6F8FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67FCE4BA-D37E-4ED4-A575-92A100E7B108}"/>
+  <xr:revisionPtr revIDLastSave="416" documentId="8_{4939A0CD-BDFC-4EBB-81BD-8799C6D6F8FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A42C501-886A-4288-8C3F-1F6F31518AF8}"/>
   <bookViews>
     <workbookView xWindow="75" yWindow="15" windowWidth="57465" windowHeight="15585" xr2:uid="{D456FA7A-7DCE-4D21-9808-82CD4ABFE24B}"/>
   </bookViews>
@@ -4720,19 +4720,19 @@
     <t>التردد النسبي {seenInLogCountOverMaxSeenInLog}٪ ({seenInLogCount} / {maxSeenInLog}).</t>
   </si>
   <si>
-    <t>غير متاح | تمت مشاهدته في {seenInLogCountOverProcessedLogsCount}٪ من السجلات ({seenInLogCount} / {processedLogsCount}). | تمت مشاهدته في {sawInLogCountOverProcessedLogsCount}٪ من السجلات ({sawInLogCount} / {processorLogsCount}).</t>
-  </si>
-  <si>
     <t>| تم تخطي خطوة واحدة. | تم تخطي {count} من الخطوات.</t>
   </si>
   <si>
     <t>الحقول المكتشفة: {detectedFields}</t>
   </si>
   <si>
-    <t>EZ Marketplace : قوالب خطوط الأنابيب : {ezMarket Pipeline Template Name}</t>
-  </si>
-  <si>
     <t>تمت مشاهدته في {seenInOverMaxSeenInLog}٪ من السجلات في العينة ({seenIn} / {maxSeenInLog})</t>
+  </si>
+  <si>
+    <t>غير متاح | تمت مشاهدته في {seenInLogCountOverProcessedLogsCount}٪ من السجلات ({seenInLogCount} / {processedLogsCount}). | تمت مشاهدته في {seenInLogCountOverProcessedLogsCount}٪ من السجلات ({seenInLogCount} / {processedLogsCount}).</t>
+  </si>
+  <si>
+    <t>EZ Marketplace : قوالب خطوط الأنابيب : {ezMarketPipelineTemplateName}</t>
   </si>
 </sst>
 </file>
@@ -5122,7 +5122,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17CA35AB-CB8B-4C3A-B66F-4EE479C36CCA}">
   <dimension ref="A1:F532"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A495" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F507" sqref="F507"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14866,7 +14868,7 @@
         <v>1518</v>
       </c>
       <c r="D443" t="s">
-        <v>1559</v>
+        <v>1562</v>
       </c>
       <c r="E443" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(JSON_Template,"VALUE",Table1[[#This Row],[fr]]),"KEY",Table1[[#This Row],[Keys]])</f>
@@ -14874,7 +14876,7 @@
       </c>
       <c r="F443" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(JSON_Template,"VALUE",Table1[[#This Row],[ar]]),"KEY",Table1[[#This Row],[Keys]])</f>
-        <v xml:space="preserve">  "N/A | Seen in {seenInLogCountOverProcessedLogsCount}% of the logs ({seenInLogCount} / {processedLogsCount}). | Seen in {seenInLogCountOverProcessedLogsCount}% of the logs ({seenInLogCount} / {processedLogsCount}).": "غير متاح | تمت مشاهدته في {seenInLogCountOverProcessedLogsCount}٪ من السجلات ({seenInLogCount} / {processedLogsCount}). | تمت مشاهدته في {sawInLogCountOverProcessedLogsCount}٪ من السجلات ({sawInLogCount} / {processorLogsCount}).",</v>
+        <v xml:space="preserve">  "N/A | Seen in {seenInLogCountOverProcessedLogsCount}% of the logs ({seenInLogCount} / {processedLogsCount}). | Seen in {seenInLogCountOverProcessedLogsCount}% of the logs ({seenInLogCount} / {processedLogsCount}).": "غير متاح | تمت مشاهدته في {seenInLogCountOverProcessedLogsCount}٪ من السجلات ({seenInLogCount} / {processedLogsCount}). | تمت مشاهدته في {seenInLogCountOverProcessedLogsCount}٪ من السجلات ({seenInLogCount} / {processedLogsCount}).",</v>
       </c>
     </row>
     <row r="444" spans="1:6" x14ac:dyDescent="0.25">
@@ -15284,7 +15286,7 @@
         <v>1529</v>
       </c>
       <c r="D462" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="E462" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(JSON_Template,"VALUE",Table1[[#This Row],[fr]]),"KEY",Table1[[#This Row],[Keys]])</f>
@@ -16054,7 +16056,7 @@
         <v>1397</v>
       </c>
       <c r="D497" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="E497" s="1" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(JSON_Template,"VALUE",Table1[[#This Row],[fr]]),"KEY",Table1[[#This Row],[Keys]])</f>
@@ -16274,7 +16276,7 @@
         <v>1398</v>
       </c>
       <c r="D507" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="E507" s="1" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(JSON_Template,"VALUE",Table1[[#This Row],[fr]]),"KEY",Table1[[#This Row],[Keys]])</f>
@@ -16282,7 +16284,7 @@
       </c>
       <c r="F507" s="1" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(JSON_Template,"VALUE",Table1[[#This Row],[ar]]),"KEY",Table1[[#This Row],[Keys]])</f>
-        <v xml:space="preserve">  "EZ Market Place : Pipeline Templates : {ezMarketPipelineTemplateName}": "EZ Marketplace : قوالب خطوط الأنابيب : {ezMarket Pipeline Template Name}",</v>
+        <v xml:space="preserve">  "EZ Market Place : Pipeline Templates : {ezMarketPipelineTemplateName}": "EZ Marketplace : قوالب خطوط الأنابيب : {ezMarketPipelineTemplateName}",</v>
       </c>
     </row>
     <row r="508" spans="1:6" x14ac:dyDescent="0.25">
@@ -16428,7 +16430,7 @@
         <v>1548</v>
       </c>
       <c r="D514" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="E514" s="1" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(JSON_Template,"VALUE",Table1[[#This Row],[fr]]),"KEY",Table1[[#This Row],[Keys]])</f>

</xml_diff>